<commit_message>
tg: sch_sth update impact forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Togo/2023/tg_sch_sth_impact_202309_1_school.xlsx
+++ b/SCH-STH/Impact assessments/Togo/2023/tg_sch_sth_impact_202309_1_school.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Togo\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657D9A0D-93C9-411D-83B4-D2D42F74BEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71F974C-513A-4640-AEBB-34DB1E142609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7150" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7150" uniqueCount="762">
   <si>
     <t>type</t>
   </si>
@@ -2487,6 +2487,36 @@
   </si>
   <si>
     <t>TOMEGBE (CMS KPADAPE)</t>
+  </si>
+  <si>
+    <t>N.DIGBE</t>
+  </si>
+  <si>
+    <t>N.TCHOUROU</t>
+  </si>
+  <si>
+    <t>L.RING</t>
+  </si>
+  <si>
+    <t>M.BOUBIAM</t>
+  </si>
+  <si>
+    <t>N.KOGNON</t>
+  </si>
+  <si>
+    <t>M.BALADO</t>
+  </si>
+  <si>
+    <t>N.TCHAWOU</t>
+  </si>
+  <si>
+    <t>N.KPASSAMBIAM</t>
+  </si>
+  <si>
+    <t>N.TCHOUROU CENTRE</t>
+  </si>
+  <si>
+    <t>N.TCHOUROU LAKAZA</t>
   </si>
 </sst>
 </file>
@@ -2902,97 +2932,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3862,8 +3802,8 @@
   <dimension ref="A1:G922"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A816" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A842" sqref="A842:XFD917"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" activeCellId="1" sqref="B1:B1048576 D1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5541,7 +5481,7 @@
         <v>76</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>586</v>
+        <v>752</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>586</v>
@@ -6786,7 +6726,7 @@
         <v>76</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>589</v>
+        <v>753</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>589</v>
@@ -8648,13 +8588,13 @@
         <v>77</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>586</v>
+        <v>752</v>
       </c>
       <c r="C336" s="3" t="s">
         <v>586</v>
       </c>
       <c r="E336" t="s">
-        <v>586</v>
+        <v>752</v>
       </c>
     </row>
     <row r="337" spans="1:5">
@@ -8662,13 +8602,13 @@
         <v>77</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>589</v>
+        <v>753</v>
       </c>
       <c r="C337" s="3" t="s">
         <v>589</v>
       </c>
       <c r="E337" t="s">
-        <v>589</v>
+        <v>753</v>
       </c>
     </row>
     <row r="338" spans="1:5">
@@ -10342,7 +10282,7 @@
         <v>78</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>404</v>
+        <v>754</v>
       </c>
       <c r="C458" s="2" t="s">
         <v>404</v>
@@ -10510,7 +10450,7 @@
         <v>78</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>412</v>
+        <v>755</v>
       </c>
       <c r="C470" s="2" t="s">
         <v>412</v>
@@ -11700,7 +11640,7 @@
         <v>78</v>
       </c>
       <c r="B555" s="2" t="s">
-        <v>487</v>
+        <v>756</v>
       </c>
       <c r="C555" s="2" t="s">
         <v>487</v>
@@ -12890,7 +12830,7 @@
         <v>78</v>
       </c>
       <c r="B640" s="2" t="s">
-        <v>550</v>
+        <v>757</v>
       </c>
       <c r="C640" s="2" t="s">
         <v>550</v>
@@ -13310,7 +13250,7 @@
         <v>78</v>
       </c>
       <c r="B670" s="2" t="s">
-        <v>575</v>
+        <v>758</v>
       </c>
       <c r="C670" s="2" t="s">
         <v>575</v>
@@ -13450,7 +13390,7 @@
         <v>78</v>
       </c>
       <c r="B680" s="2" t="s">
-        <v>583</v>
+        <v>759</v>
       </c>
       <c r="C680" s="2" t="s">
         <v>583</v>
@@ -13492,13 +13432,13 @@
         <v>78</v>
       </c>
       <c r="B683" s="2" t="s">
-        <v>586</v>
+        <v>752</v>
       </c>
       <c r="C683" s="2" t="s">
         <v>586</v>
       </c>
       <c r="F683" t="s">
-        <v>586</v>
+        <v>752</v>
       </c>
     </row>
     <row r="684" spans="1:6">
@@ -13512,7 +13452,7 @@
         <v>587</v>
       </c>
       <c r="F684" t="s">
-        <v>586</v>
+        <v>752</v>
       </c>
     </row>
     <row r="685" spans="1:6">
@@ -13520,13 +13460,13 @@
         <v>78</v>
       </c>
       <c r="B685" s="2" t="s">
-        <v>588</v>
+        <v>760</v>
       </c>
       <c r="C685" s="2" t="s">
         <v>588</v>
       </c>
       <c r="F685" t="s">
-        <v>589</v>
+        <v>753</v>
       </c>
     </row>
     <row r="686" spans="1:6">
@@ -13534,13 +13474,13 @@
         <v>78</v>
       </c>
       <c r="B686" s="2" t="s">
-        <v>590</v>
+        <v>761</v>
       </c>
       <c r="C686" s="2" t="s">
         <v>590</v>
       </c>
       <c r="F686" t="s">
-        <v>589</v>
+        <v>753</v>
       </c>
     </row>
     <row r="687" spans="1:6">

</xml_diff>